<commit_message>
plein de choses cool
</commit_message>
<xml_diff>
--- a/BADGOTRON/Gestion_FLASH.xlsx
+++ b/BADGOTRON/Gestion_FLASH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17145" windowHeight="10320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17145" windowHeight="10320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -913,11 +913,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="4">
+  <numFmts count="6">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.000000_);_(* \(#,##0.000000\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.0000000_);_(* \(#,##0.0000000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.00000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -1166,7 +1168,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -1186,11 +1188,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1241,6 +1239,21 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1271,24 +1284,14 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="170" fontId="6" fillId="12" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1573,8 +1576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1601,14 +1604,14 @@
       <c r="B1" s="5">
         <v>21824</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="16">
+      <c r="E1" s="15">
         <f>16*1024*1024</f>
         <v>16777216</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="15" t="s">
         <v>47</v>
       </c>
       <c r="M1" s="2" t="s">
@@ -1624,19 +1627,19 @@
       </c>
       <c r="B2" s="2">
         <f>B43</f>
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="15">
         <f>E1/E3</f>
         <v>512</v>
       </c>
-      <c r="F2" s="16"/>
+      <c r="F2" s="15"/>
       <c r="M2" s="2" t="s">
         <v>20</v>
       </c>
@@ -1650,19 +1653,19 @@
       </c>
       <c r="B3" s="4">
         <f>B1*B2</f>
-        <v>5936128</v>
+        <v>6634496</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="16">
+      <c r="E3" s="15">
         <f>4096*8</f>
         <v>32768</v>
       </c>
-      <c r="F3" s="16"/>
+      <c r="F3" s="15"/>
       <c r="M3" s="2" t="s">
         <v>22</v>
       </c>
@@ -1674,18 +1677,18 @@
       <c r="A4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="84">
         <f>B1/B5</f>
-        <v>181.86666666666667</v>
-      </c>
-      <c r="D4" s="16" t="s">
+        <v>203.96261682242991</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="E4" s="16">
+      <c r="E4" s="15">
         <f>E3/8</f>
         <v>4096</v>
       </c>
-      <c r="F4" s="16"/>
+      <c r="F4" s="15"/>
       <c r="M4" s="2" t="s">
         <v>23</v>
       </c>
@@ -1697,8 +1700,8 @@
       <c r="A5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="17">
-        <v>120</v>
+      <c r="B5" s="83">
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
@@ -1738,7 +1741,7 @@
       </c>
       <c r="E8" s="3">
         <f>E2-B10-B4</f>
-        <v>298.13333333333333</v>
+        <v>276.03738317757006</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>25</v>
@@ -1763,14 +1766,14 @@
       </c>
       <c r="E9" s="3">
         <f>E2-E8</f>
-        <v>213.86666666666667</v>
+        <v>235.96261682242994</v>
       </c>
       <c r="H9" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I9" s="6">
         <f>B3/8+B9</f>
-        <v>1789568</v>
+        <v>1876864</v>
       </c>
       <c r="M9" s="2" t="s">
         <v>26</v>
@@ -1804,7 +1807,7 @@
       <c r="A11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>682</v>
       </c>
       <c r="H11" s="2" t="s">
@@ -1812,7 +1815,7 @@
       </c>
       <c r="I11" s="8">
         <f>I9/E1</f>
-        <v>0.10666656494140625</v>
+        <v>0.11186981201171875</v>
       </c>
       <c r="M11" s="2" t="s">
         <v>19</v>
@@ -1837,7 +1840,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="17" t="s">
         <v>96</v>
       </c>
       <c r="B14" s="6"/>
@@ -1860,10 +1863,10 @@
       <c r="D20" s="6"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="B26" s="15"/>
+      <c r="B26" s="66"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
@@ -1902,7 +1905,7 @@
         <v>33</v>
       </c>
       <c r="B31" s="10">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -1934,7 +1937,7 @@
         <v>37</v>
       </c>
       <c r="B35" s="10">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -1999,7 +2002,7 @@
       </c>
       <c r="B43" s="12">
         <f>SUM(B27:B42)</f>
-        <v>272</v>
+        <v>304</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>47</v>
@@ -2011,7 +2014,7 @@
       </c>
       <c r="B44" s="14">
         <f>B43/8</f>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>48</v>
@@ -2031,7 +2034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -2045,1090 +2048,1090 @@
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="68" t="s">
+      <c r="A2" s="71" t="s">
         <v>278</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="27" t="s">
+      <c r="D2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="F2" s="27" t="s">
+      <c r="F2" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="G2" s="27" t="s">
+      <c r="G2" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H2" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="J2" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="28" t="s">
+      <c r="H2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J2" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="26" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="69"/>
-      <c r="B3" s="29" t="s">
+      <c r="A3" s="72"/>
+      <c r="B3" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="G3" s="30" t="s">
+      <c r="G3" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="H3" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="I3" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J3" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="K3" s="31" t="s">
+      <c r="H3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="29" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="70" t="s">
+      <c r="A4" s="73" t="s">
         <v>279</v>
       </c>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="39" t="s">
+      <c r="C4" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="D4" s="39" t="s">
+      <c r="D4" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="37" t="s">
         <v>100</v>
       </c>
-      <c r="F4" s="39" t="s">
+      <c r="F4" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="G4" s="39" t="s">
+      <c r="G4" s="37" t="s">
         <v>102</v>
       </c>
-      <c r="H4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="J4" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="K4" s="40" t="s">
+      <c r="H4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="K4" s="38" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="71"/>
-      <c r="B5" s="41" t="s">
+      <c r="A5" s="74"/>
+      <c r="B5" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="D5" s="42" t="s">
+      <c r="D5" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="40" t="s">
         <v>106</v>
       </c>
-      <c r="F5" s="42" t="s">
+      <c r="F5" s="40" t="s">
         <v>107</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="40" t="s">
         <v>108</v>
       </c>
-      <c r="H5" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="K5" s="43" t="s">
+      <c r="H5" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I5" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="J5" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="41" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="75" t="s">
         <v>280</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="42" t="s">
         <v>60</v>
       </c>
-      <c r="C6" s="45" t="s">
+      <c r="C6" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="E6" s="45" t="s">
+      <c r="E6" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="G6" s="45" t="s">
+      <c r="G6" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="H6" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="I6" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="J6" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="46" t="s">
+      <c r="H6" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="I6" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="J6" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="K6" s="44" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="73"/>
-      <c r="B7" s="47" t="s">
+      <c r="A7" s="76"/>
+      <c r="B7" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="C7" s="48" t="s">
+      <c r="C7" s="46" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="48" t="s">
+      <c r="D7" s="46" t="s">
         <v>117</v>
       </c>
-      <c r="E7" s="48" t="s">
+      <c r="E7" s="46" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="48" t="s">
+      <c r="F7" s="46" t="s">
         <v>119</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="H7" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="J7" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="K7" s="49" t="s">
+      <c r="H7" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="K7" s="47" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="77" t="s">
         <v>281</v>
       </c>
-      <c r="B8" s="56" t="s">
+      <c r="B8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="55" t="s">
         <v>122</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="55" t="s">
         <v>123</v>
       </c>
-      <c r="E8" s="57" t="s">
+      <c r="E8" s="55" t="s">
         <v>124</v>
       </c>
-      <c r="F8" s="57" t="s">
+      <c r="F8" s="55" t="s">
         <v>125</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="55" t="s">
         <v>126</v>
       </c>
-      <c r="H8" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="I8" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="J8" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="K8" s="58" t="s">
+      <c r="H8" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I8" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="J8" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K8" s="56" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="75"/>
-      <c r="B9" s="59" t="s">
+      <c r="A9" s="78"/>
+      <c r="B9" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="58" t="s">
         <v>128</v>
       </c>
-      <c r="D9" s="60" t="s">
+      <c r="D9" s="58" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="60" t="s">
+      <c r="E9" s="58" t="s">
         <v>130</v>
       </c>
-      <c r="F9" s="60" t="s">
+      <c r="F9" s="58" t="s">
         <v>131</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="58" t="s">
         <v>132</v>
       </c>
-      <c r="H9" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="I9" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="J9" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="61" t="s">
+      <c r="H9" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="J9" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="59" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="76" t="s">
+      <c r="A10" s="79" t="s">
         <v>282</v>
       </c>
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="61" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="61" t="s">
         <v>135</v>
       </c>
-      <c r="E10" s="63" t="s">
+      <c r="E10" s="61" t="s">
         <v>136</v>
       </c>
-      <c r="F10" s="63" t="s">
+      <c r="F10" s="61" t="s">
         <v>137</v>
       </c>
-      <c r="G10" s="63" t="s">
+      <c r="G10" s="61" t="s">
         <v>138</v>
       </c>
-      <c r="H10" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="I10" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="K10" s="64" t="s">
+      <c r="H10" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="62" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="77"/>
-      <c r="B11" s="65" t="s">
+      <c r="A11" s="80"/>
+      <c r="B11" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="64" t="s">
         <v>141</v>
       </c>
-      <c r="E11" s="66" t="s">
+      <c r="E11" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="F11" s="66" t="s">
+      <c r="F11" s="64" t="s">
         <v>143</v>
       </c>
-      <c r="G11" s="66" t="s">
+      <c r="G11" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="H11" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="I11" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="J11" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="K11" s="67" t="s">
+      <c r="H11" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="J11" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="K11" s="65" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="78" t="s">
+      <c r="A12" s="67" t="s">
         <v>283</v>
       </c>
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="31" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="33" t="s">
+      <c r="D12" s="31" t="s">
         <v>147</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" s="31" t="s">
         <v>148</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="31" t="s">
         <v>149</v>
       </c>
-      <c r="G12" s="33" t="s">
+      <c r="G12" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="H12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="K12" s="34" t="s">
+      <c r="H12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="32" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="79"/>
-      <c r="B13" s="35" t="s">
+      <c r="A13" s="68"/>
+      <c r="B13" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="36" t="s">
+      <c r="C13" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="D13" s="36" t="s">
+      <c r="D13" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="G13" s="36" t="s">
+      <c r="G13" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="H13" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="J13" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="K13" s="37" t="s">
+      <c r="H13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="J13" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="K13" s="35" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="81" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="50" t="s">
+      <c r="B14" s="48" t="s">
         <v>68</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="49" t="s">
         <v>158</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="49" t="s">
         <v>159</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="49" t="s">
         <v>160</v>
       </c>
-      <c r="F14" s="51" t="s">
+      <c r="F14" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="49" t="s">
         <v>162</v>
       </c>
-      <c r="H14" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="I14" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="J14" s="51" t="s">
-        <v>57</v>
-      </c>
-      <c r="K14" s="52" t="s">
+      <c r="H14" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="J14" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="K14" s="50" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
-      <c r="B15" s="53" t="s">
+      <c r="A15" s="82"/>
+      <c r="B15" s="51" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="54" t="s">
+      <c r="C15" s="52" t="s">
         <v>164</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="52" t="s">
         <v>165</v>
       </c>
-      <c r="E15" s="54" t="s">
+      <c r="E15" s="52" t="s">
         <v>166</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="52" t="s">
         <v>167</v>
       </c>
-      <c r="G15" s="54" t="s">
+      <c r="G15" s="52" t="s">
         <v>168</v>
       </c>
-      <c r="H15" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="54" t="s">
-        <v>57</v>
-      </c>
-      <c r="K15" s="55" t="s">
+      <c r="H15" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" s="52" t="s">
+        <v>57</v>
+      </c>
+      <c r="K15" s="53" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="68" t="s">
+      <c r="A16" s="71" t="s">
         <v>285</v>
       </c>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F16" s="27" t="s">
+      <c r="F16" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="G16" s="27" t="s">
+      <c r="G16" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="H16" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="I16" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="J16" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="K16" s="28" t="s">
+      <c r="H16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="J16" s="25" t="s">
+        <v>57</v>
+      </c>
+      <c r="K16" s="26" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="69"/>
-      <c r="B17" s="29" t="s">
+      <c r="A17" s="72"/>
+      <c r="B17" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="C17" s="30" t="s">
+      <c r="C17" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="28" t="s">
         <v>179</v>
       </c>
-      <c r="G17" s="30" t="s">
+      <c r="G17" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="H17" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="I17" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="J17" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="K17" s="31" t="s">
+      <c r="H17" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="I17" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="K17" s="29" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="70" t="s">
+      <c r="A18" s="73" t="s">
         <v>286</v>
       </c>
-      <c r="B18" s="38" t="s">
+      <c r="B18" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="D18" s="39" t="s">
+      <c r="D18" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="E18" s="39" t="s">
+      <c r="E18" s="37" t="s">
         <v>184</v>
       </c>
-      <c r="F18" s="39" t="s">
+      <c r="F18" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="H18" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="I18" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="J18" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="K18" s="40" t="s">
+      <c r="H18" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="37" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="38" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="71"/>
-      <c r="B19" s="41" t="s">
+      <c r="A19" s="74"/>
+      <c r="B19" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="42" t="s">
+      <c r="C19" s="40" t="s">
         <v>188</v>
       </c>
-      <c r="D19" s="42" t="s">
+      <c r="D19" s="40" t="s">
         <v>189</v>
       </c>
-      <c r="E19" s="42" t="s">
+      <c r="E19" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="F19" s="42" t="s">
+      <c r="F19" s="40" t="s">
         <v>191</v>
       </c>
-      <c r="G19" s="42" t="s">
+      <c r="G19" s="40" t="s">
         <v>192</v>
       </c>
-      <c r="H19" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="J19" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" s="43" t="s">
+      <c r="H19" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="I19" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="J19" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="41" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="72" t="s">
+      <c r="A20" s="75" t="s">
         <v>287</v>
       </c>
-      <c r="B20" s="44" t="s">
+      <c r="B20" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="43" t="s">
         <v>194</v>
       </c>
-      <c r="D20" s="45" t="s">
+      <c r="D20" s="43" t="s">
         <v>195</v>
       </c>
-      <c r="E20" s="45" t="s">
+      <c r="E20" s="43" t="s">
         <v>196</v>
       </c>
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="43" t="s">
         <v>197</v>
       </c>
-      <c r="G20" s="45" t="s">
+      <c r="G20" s="43" t="s">
         <v>198</v>
       </c>
-      <c r="H20" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="I20" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="J20" s="45" t="s">
-        <v>57</v>
-      </c>
-      <c r="K20" s="46" t="s">
+      <c r="H20" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="K20" s="44" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="73"/>
-      <c r="B21" s="47" t="s">
+      <c r="A21" s="76"/>
+      <c r="B21" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="46" t="s">
         <v>200</v>
       </c>
-      <c r="D21" s="48" t="s">
+      <c r="D21" s="46" t="s">
         <v>201</v>
       </c>
-      <c r="E21" s="48" t="s">
+      <c r="E21" s="46" t="s">
         <v>202</v>
       </c>
-      <c r="F21" s="48" t="s">
+      <c r="F21" s="46" t="s">
         <v>203</v>
       </c>
-      <c r="G21" s="48" t="s">
+      <c r="G21" s="46" t="s">
         <v>204</v>
       </c>
-      <c r="H21" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="I21" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="J21" s="48" t="s">
-        <v>57</v>
-      </c>
-      <c r="K21" s="49" t="s">
+      <c r="H21" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="J21" s="46" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="47" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="74" t="s">
+      <c r="A22" s="77" t="s">
         <v>288</v>
       </c>
-      <c r="B22" s="56" t="s">
+      <c r="B22" s="54" t="s">
         <v>82</v>
       </c>
-      <c r="C22" s="57" t="s">
+      <c r="C22" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="D22" s="57" t="s">
+      <c r="D22" s="55" t="s">
         <v>207</v>
       </c>
-      <c r="E22" s="57" t="s">
+      <c r="E22" s="55" t="s">
         <v>208</v>
       </c>
-      <c r="F22" s="57" t="s">
+      <c r="F22" s="55" t="s">
         <v>209</v>
       </c>
-      <c r="G22" s="57" t="s">
+      <c r="G22" s="55" t="s">
         <v>210</v>
       </c>
-      <c r="H22" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="I22" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="J22" s="57" t="s">
-        <v>57</v>
-      </c>
-      <c r="K22" s="58" t="s">
+      <c r="H22" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="J22" s="55" t="s">
+        <v>57</v>
+      </c>
+      <c r="K22" s="56" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="75"/>
-      <c r="B23" s="59" t="s">
+      <c r="A23" s="78"/>
+      <c r="B23" s="57" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="60" t="s">
+      <c r="C23" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="D23" s="60" t="s">
+      <c r="D23" s="58" t="s">
         <v>213</v>
       </c>
-      <c r="E23" s="60" t="s">
+      <c r="E23" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="F23" s="60" t="s">
+      <c r="F23" s="58" t="s">
         <v>215</v>
       </c>
-      <c r="G23" s="60" t="s">
+      <c r="G23" s="58" t="s">
         <v>216</v>
       </c>
-      <c r="H23" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="I23" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="J23" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="K23" s="61" t="s">
+      <c r="H23" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="I23" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="J23" s="58" t="s">
+        <v>57</v>
+      </c>
+      <c r="K23" s="59" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="79" t="s">
         <v>289</v>
       </c>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="60" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="63" t="s">
+      <c r="C24" s="61" t="s">
         <v>218</v>
       </c>
-      <c r="D24" s="63" t="s">
+      <c r="D24" s="61" t="s">
         <v>219</v>
       </c>
-      <c r="E24" s="63" t="s">
+      <c r="E24" s="61" t="s">
         <v>220</v>
       </c>
-      <c r="F24" s="63" t="s">
+      <c r="F24" s="61" t="s">
         <v>221</v>
       </c>
-      <c r="G24" s="63" t="s">
+      <c r="G24" s="61" t="s">
         <v>222</v>
       </c>
-      <c r="H24" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="I24" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="J24" s="63" t="s">
-        <v>57</v>
-      </c>
-      <c r="K24" s="64" t="s">
+      <c r="H24" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="I24" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="J24" s="61" t="s">
+        <v>57</v>
+      </c>
+      <c r="K24" s="62" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="77"/>
-      <c r="B25" s="65" t="s">
+      <c r="A25" s="80"/>
+      <c r="B25" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="66" t="s">
+      <c r="C25" s="64" t="s">
         <v>224</v>
       </c>
-      <c r="D25" s="66" t="s">
+      <c r="D25" s="64" t="s">
         <v>225</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="64" t="s">
         <v>226</v>
       </c>
-      <c r="F25" s="66" t="s">
+      <c r="F25" s="64" t="s">
         <v>227</v>
       </c>
-      <c r="G25" s="66" t="s">
+      <c r="G25" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="H25" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="I25" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="J25" s="66" t="s">
-        <v>57</v>
-      </c>
-      <c r="K25" s="67" t="s">
+      <c r="H25" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="I25" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="J25" s="64" t="s">
+        <v>57</v>
+      </c>
+      <c r="K25" s="65" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="78" t="s">
+      <c r="A26" s="67" t="s">
         <v>290</v>
       </c>
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="31" t="s">
         <v>230</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G26" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="H26" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="I26" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="J26" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="K26" s="34" t="s">
+      <c r="H26" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="I26" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="J26" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="K26" s="32" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="79"/>
-      <c r="B27" s="35" t="s">
+      <c r="A27" s="68"/>
+      <c r="B27" s="33" t="s">
         <v>87</v>
       </c>
-      <c r="C27" s="36" t="s">
+      <c r="C27" s="34" t="s">
         <v>236</v>
       </c>
-      <c r="D27" s="36" t="s">
+      <c r="D27" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="34" t="s">
         <v>238</v>
       </c>
-      <c r="F27" s="36" t="s">
+      <c r="F27" s="34" t="s">
         <v>239</v>
       </c>
-      <c r="G27" s="36" t="s">
+      <c r="G27" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="H27" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="I27" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="J27" s="36" t="s">
-        <v>57</v>
-      </c>
-      <c r="K27" s="37" t="s">
+      <c r="H27" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="I27" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="K27" s="35" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="82" t="s">
+      <c r="A28" s="69" t="s">
         <v>291</v>
       </c>
-      <c r="B28" s="20" t="s">
+      <c r="B28" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="19" t="s">
         <v>242</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="19" t="s">
         <v>243</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="19" t="s">
         <v>244</v>
       </c>
-      <c r="F28" s="21" t="s">
+      <c r="F28" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="G28" s="21" t="s">
+      <c r="G28" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="H28" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I28" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="J28" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K28" s="22" t="s">
+      <c r="H28" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J28" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K28" s="20" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="83"/>
-      <c r="B29" s="23" t="s">
+      <c r="A29" s="70"/>
+      <c r="B29" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="D29" s="24" t="s">
+      <c r="D29" s="22" t="s">
         <v>249</v>
       </c>
-      <c r="E29" s="24" t="s">
+      <c r="E29" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="F29" s="24" t="s">
+      <c r="F29" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="H29" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I29" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="J29" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="K29" s="25" t="s">
+      <c r="H29" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I29" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K29" s="23" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="82" t="s">
+      <c r="A30" s="69" t="s">
         <v>292</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D30" s="19" t="s">
         <v>255</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="19" t="s">
         <v>256</v>
       </c>
-      <c r="F30" s="21" t="s">
+      <c r="F30" s="19" t="s">
         <v>257</v>
       </c>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="19" t="s">
         <v>258</v>
       </c>
-      <c r="H30" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I30" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="J30" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K30" s="22" t="s">
+      <c r="H30" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I30" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J30" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K30" s="20" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="83"/>
-      <c r="B31" s="23" t="s">
+      <c r="A31" s="70"/>
+      <c r="B31" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="C31" s="24" t="s">
+      <c r="C31" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="D31" s="24" t="s">
+      <c r="D31" s="22" t="s">
         <v>261</v>
       </c>
-      <c r="E31" s="24" t="s">
+      <c r="E31" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="F31" s="24" t="s">
+      <c r="F31" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G31" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="H31" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I31" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="J31" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="K31" s="25" t="s">
+      <c r="H31" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K31" s="23" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="82" t="s">
+      <c r="A32" s="69" t="s">
         <v>293</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="D32" s="21" t="s">
+      <c r="D32" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="E32" s="21" t="s">
+      <c r="E32" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="F32" s="21" t="s">
+      <c r="F32" s="19" t="s">
         <v>269</v>
       </c>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="19" t="s">
         <v>270</v>
       </c>
-      <c r="H32" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I32" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="J32" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="K32" s="22" t="s">
+      <c r="H32" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="I32" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="J32" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K32" s="20" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="83"/>
-      <c r="B33" s="23" t="s">
+      <c r="A33" s="70"/>
+      <c r="B33" s="21" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="24" t="s">
+      <c r="C33" s="22" t="s">
         <v>272</v>
       </c>
-      <c r="D33" s="24" t="s">
+      <c r="D33" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="F33" s="24" t="s">
+      <c r="F33" s="22" t="s">
         <v>275</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="H33" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="I33" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="J33" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="K33" s="25" t="s">
+      <c r="H33" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I33" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="K33" s="23" t="s">
         <v>277</v>
       </c>
     </row>

</xml_diff>